<commit_message>
test automation -- server side fixes
</commit_message>
<xml_diff>
--- a/wearable-school-server/EpisodePlan-SingleWatch.xlsx
+++ b/wearable-school-server/EpisodePlan-SingleWatch.xlsx
@@ -559,7 +559,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,10 +581,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,8 +703,8 @@
   </sheetPr>
   <dimension ref="A1:AF105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -717,11 +713,11 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.57085020242915"/>
@@ -729,7 +725,7 @@
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +793,7 @@
       <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AA1" s="3" t="s">
@@ -823,23 +819,23 @@
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7" t="str">
+      <c r="C2" s="6" t="str">
         <f aca="false">IF(D2="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="E2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="1" t="n">
@@ -887,25 +883,25 @@
       <c r="W2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="9" t="n">
+      <c r="AA2" s="8" t="n">
         <v>650</v>
       </c>
-      <c r="AB2" s="9" t="n">
+      <c r="AB2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AC2" s="9" t="n">
+      <c r="AC2" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="AD2" s="9" t="n">
+      <c r="AD2" s="8" t="n">
         <v>650</v>
       </c>
-      <c r="AE2" s="9" t="n">
+      <c r="AE2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AF2" s="9" t="n">
+      <c r="AF2" s="8" t="n">
         <v>18</v>
       </c>
     </row>
@@ -913,23 +909,23 @@
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="str">
+      <c r="C3" s="6" t="str">
         <f aca="false">IF(D3="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="E3" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I3" s="1" t="n">
@@ -956,21 +952,21 @@
         <f aca="false">VLOOKUP($H3,$Z$2:$AF$9,7,0)</f>
         <v>32</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="9" t="n">
+      <c r="AA3" s="8" t="n">
         <v>650</v>
       </c>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="9" t="n">
+      <c r="AC3" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="AD3" s="9" t="n">
+      <c r="AD3" s="8" t="n">
         <v>650</v>
       </c>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="9" t="n">
+      <c r="AF3" s="8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -978,23 +974,23 @@
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="str">
+      <c r="C4" s="6" t="str">
         <f aca="false">IF(D4="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="E4" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="1" t="n">
@@ -1021,21 +1017,21 @@
         <f aca="false">VLOOKUP($H4,$Z$2:$AF$9,7,0)</f>
         <v>330</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="Z4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AA4" s="9" t="n">
+      <c r="AA4" s="8" t="n">
         <v>100</v>
       </c>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="9" t="n">
+      <c r="AC4" s="8" t="n">
         <v>780</v>
       </c>
-      <c r="AD4" s="9" t="n">
+      <c r="AD4" s="8" t="n">
         <v>100</v>
       </c>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="9" t="n">
+      <c r="AF4" s="8" t="n">
         <v>330</v>
       </c>
     </row>
@@ -1043,23 +1039,23 @@
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C5" s="6" t="str">
         <f aca="false">IF(D5="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="E5" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="1" t="n">
@@ -1086,21 +1082,21 @@
         <f aca="false">VLOOKUP($H5,$Z$2:$AF$9,7,0)</f>
         <v>420</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="Z5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AA5" s="9" t="n">
+      <c r="AA5" s="8" t="n">
         <v>90</v>
       </c>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="9" t="n">
+      <c r="AC5" s="8" t="n">
         <v>850</v>
       </c>
-      <c r="AD5" s="9" t="n">
+      <c r="AD5" s="8" t="n">
         <v>100</v>
       </c>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="9" t="n">
+      <c r="AF5" s="8" t="n">
         <v>420</v>
       </c>
     </row>
@@ -1108,23 +1104,23 @@
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="7" t="str">
+      <c r="C6" s="6" t="str">
         <f aca="false">IF(D6="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="E6" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="1" t="n">
@@ -1151,21 +1147,21 @@
         <f aca="false">VLOOKUP($H6,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="Z6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AA6" s="9" t="n">
+      <c r="AA6" s="8" t="n">
         <v>400</v>
       </c>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="9" t="n">
+      <c r="AC6" s="8" t="n">
         <v>240</v>
       </c>
-      <c r="AD6" s="9" t="n">
+      <c r="AD6" s="8" t="n">
         <v>440</v>
       </c>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="9" t="n">
+      <c r="AF6" s="8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1173,23 +1169,23 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="str">
+      <c r="C7" s="6" t="str">
         <f aca="false">IF(D7="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="E7" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I7" s="1" t="n">
@@ -1216,21 +1212,21 @@
         <f aca="false">VLOOKUP($H7,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="Z7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AA7" s="9" t="n">
+      <c r="AA7" s="8" t="n">
         <v>350</v>
       </c>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="9" t="n">
+      <c r="AC7" s="8" t="n">
         <v>250</v>
       </c>
-      <c r="AD7" s="9" t="n">
+      <c r="AD7" s="8" t="n">
         <v>370</v>
       </c>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="9" t="n">
+      <c r="AF7" s="8" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1238,23 +1234,23 @@
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="6" t="str">
         <f aca="false">IF(D8="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="E8" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I8" s="1" t="n">
@@ -1281,49 +1277,49 @@
         <f aca="false">VLOOKUP($H8,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="Z8" s="8" t="s">
+      <c r="Z8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AA8" s="9" t="n">
+      <c r="AA8" s="8" t="n">
         <v>400</v>
       </c>
-      <c r="AB8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="9" t="n">
+      <c r="AB8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="8" t="n">
         <v>240</v>
       </c>
-      <c r="AD8" s="9" t="n">
+      <c r="AD8" s="8" t="n">
         <v>440</v>
       </c>
-      <c r="AE8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="9" t="n">
+      <c r="AE8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="8" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="7" t="str">
+      <c r="C9" s="6" t="str">
         <f aca="false">IF(D9="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentA</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="E9" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="1" t="n">
@@ -1350,7 +1346,7 @@
         <f aca="false">VLOOKUP($H9,$Z$2:$AF$9,7,0)</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="8" t="s">
+      <c r="Z9" s="7" t="s">
         <v>39</v>
       </c>
       <c r="AA9" s="1"/>
@@ -1360,27 +1356,27 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="10" t="str">
+      <c r="C10" s="9" t="str">
         <f aca="false">IF(D10="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="D10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="1" t="n">
@@ -1408,27 +1404,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="str">
+      <c r="C11" s="9" t="str">
         <f aca="false">IF(D11="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11" t="s">
+      <c r="D11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F11" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>27</v>
       </c>
       <c r="I11" s="1" t="n">
@@ -1456,27 +1452,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="10" t="str">
+      <c r="C12" s="9" t="str">
         <f aca="false">IF(D12="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G12" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="1" t="n">
@@ -1504,27 +1500,27 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="10" t="str">
+      <c r="C13" s="9" t="str">
         <f aca="false">IF(D13="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="D13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G13" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="1" t="n">
@@ -1552,27 +1548,27 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="10" t="str">
+      <c r="C14" s="9" t="str">
         <f aca="false">IF(D14="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G14" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="D14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="1" t="n">
@@ -1600,27 +1596,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="10" t="str">
+      <c r="C15" s="9" t="str">
         <f aca="false">IF(D15="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="11" t="s">
+      <c r="D15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G15" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I15" s="1" t="n">
@@ -1648,27 +1644,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="10" t="str">
+      <c r="C16" s="9" t="str">
         <f aca="false">IF(D16="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="D16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G16" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I16" s="1" t="n">
@@ -1695,7 +1691,7 @@
         <f aca="false">VLOOKUP($H16,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="Q16" s="12" t="n">
+      <c r="Q16" s="11" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1703,23 +1699,23 @@
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="10" t="str">
+      <c r="C17" s="9" t="str">
         <f aca="false">IF(D17="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11" t="s">
+      <c r="D17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G17" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="1" t="n">
@@ -1754,23 +1750,23 @@
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="13" t="str">
+      <c r="C18" s="12" t="str">
         <f aca="false">IF(D18="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G18" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="14" t="s">
+      <c r="D18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="1" t="n">
@@ -1805,23 +1801,23 @@
       <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="13" t="str">
+      <c r="C19" s="12" t="str">
         <f aca="false">IF(D19="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G19" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="14" t="s">
+      <c r="D19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I19" s="1" t="n">
@@ -1856,23 +1852,23 @@
       <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="13" t="str">
+      <c r="C20" s="12" t="str">
         <f aca="false">IF(D20="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G20" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="14" t="s">
+      <c r="D20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G20" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I20" s="1" t="n">
@@ -1907,23 +1903,23 @@
       <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="13" t="str">
+      <c r="C21" s="12" t="str">
         <f aca="false">IF(D21="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G21" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="14" t="s">
+      <c r="D21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G21" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I21" s="1" t="n">
@@ -1958,23 +1954,23 @@
       <c r="B22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="13" t="str">
+      <c r="C22" s="12" t="str">
         <f aca="false">IF(D22="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G22" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="14" t="s">
+      <c r="D22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="1" t="n">
@@ -2006,23 +2002,23 @@
       <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="13" t="str">
+      <c r="C23" s="12" t="str">
         <f aca="false">IF(D23="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G23" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="14" t="s">
+      <c r="D23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I23" s="1" t="n">
@@ -2054,23 +2050,23 @@
       <c r="B24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="13" t="str">
+      <c r="C24" s="12" t="str">
         <f aca="false">IF(D24="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G24" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="14" t="s">
+      <c r="D24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G24" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>37</v>
       </c>
       <c r="I24" s="1" t="n">
@@ -2102,23 +2098,23 @@
       <c r="B25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="13" t="str">
+      <c r="C25" s="12" t="str">
         <f aca="false">IF(D25="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G25" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="14" t="s">
+      <c r="D25" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>39</v>
       </c>
       <c r="I25" s="1" t="n">
@@ -2150,23 +2146,23 @@
       <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="7" t="str">
+      <c r="C26" s="6" t="str">
         <f aca="false">IF(D26="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="D26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="1" t="n">
@@ -2193,34 +2189,34 @@
         <f aca="false">VLOOKUP($H26,$Z$2:$AF$9,7,0)</f>
         <v>18</v>
       </c>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
-      <c r="AA26" s="15"/>
-      <c r="AB26" s="16"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="7" t="str">
+      <c r="C27" s="6" t="str">
         <f aca="false">IF(D27="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G27" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="D27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I27" s="1" t="n">
@@ -2247,34 +2243,34 @@
         <f aca="false">VLOOKUP($H27,$Z$2:$AF$9,7,0)</f>
         <v>32</v>
       </c>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-      <c r="AA27" s="15"/>
-      <c r="AB27" s="16"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="7" t="str">
+      <c r="C28" s="6" t="str">
         <f aca="false">IF(D28="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G28" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8" t="s">
+      <c r="D28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I28" s="1" t="n">
@@ -2301,34 +2297,34 @@
         <f aca="false">VLOOKUP($H28,$Z$2:$AF$9,7,0)</f>
         <v>330</v>
       </c>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="15"/>
-      <c r="AB28" s="16"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="7" t="str">
+      <c r="C29" s="6" t="str">
         <f aca="false">IF(D29="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G29" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="D29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="1" t="n">
@@ -2355,34 +2351,34 @@
         <f aca="false">VLOOKUP($H29,$Z$2:$AF$9,7,0)</f>
         <v>420</v>
       </c>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
-      <c r="AA29" s="15"/>
-      <c r="AB29" s="16"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="7" t="str">
+      <c r="C30" s="6" t="str">
         <f aca="false">IF(D30="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" s="8" t="s">
+      <c r="D30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="1" t="n">
@@ -2409,34 +2405,34 @@
         <f aca="false">VLOOKUP($H30,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-      <c r="AA30" s="15"/>
-      <c r="AB30" s="16"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+      <c r="AB30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="7" t="str">
+      <c r="C31" s="6" t="str">
         <f aca="false">IF(D31="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G31" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H31" s="8" t="s">
+      <c r="D31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I31" s="1" t="n">
@@ -2463,34 +2459,34 @@
         <f aca="false">VLOOKUP($H31,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="15"/>
-      <c r="AB31" s="16"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14"/>
+      <c r="AB31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="7" t="str">
+      <c r="C32" s="6" t="str">
         <f aca="false">IF(D32="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="8" t="s">
+      <c r="D32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I32" s="1" t="n">
@@ -2517,34 +2513,34 @@
         <f aca="false">VLOOKUP($H32,$Z$2:$AF$9,7,0)</f>
         <v>200</v>
       </c>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="15"/>
-      <c r="AB32" s="16"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="14"/>
+      <c r="AB32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="7" t="str">
+      <c r="C33" s="6" t="str">
         <f aca="false">IF(D33="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G33" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" s="8" t="s">
+      <c r="D33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="1" t="n">
@@ -2571,34 +2567,34 @@
         <f aca="false">VLOOKUP($H33,$Z$2:$AF$9,7,0)</f>
         <v>0</v>
       </c>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="15"/>
-      <c r="AB33" s="16"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="14"/>
+      <c r="AB33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="10" t="str">
+      <c r="C34" s="9" t="str">
         <f aca="false">IF(D34="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G34" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="11" t="s">
+      <c r="D34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G34" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I34" s="1" t="n">
@@ -2630,23 +2626,23 @@
       <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="10" t="str">
+      <c r="C35" s="9" t="str">
         <f aca="false">IF(D35="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G35" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" s="11" t="s">
+      <c r="D35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G35" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="10" t="s">
         <v>27</v>
       </c>
       <c r="I35" s="1" t="n">
@@ -2678,23 +2674,23 @@
       <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="10" t="str">
+      <c r="C36" s="9" t="str">
         <f aca="false">IF(D36="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G36" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H36" s="11" t="s">
+      <c r="D36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G36" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>29</v>
       </c>
       <c r="I36" s="1" t="n">
@@ -2726,23 +2722,23 @@
       <c r="B37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="10" t="str">
+      <c r="C37" s="9" t="str">
         <f aca="false">IF(D37="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G37" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" s="11" t="s">
+      <c r="D37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G37" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I37" s="1" t="n">
@@ -2774,23 +2770,23 @@
       <c r="B38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="10" t="str">
+      <c r="C38" s="9" t="str">
         <f aca="false">IF(D38="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G38" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" s="11" t="s">
+      <c r="D38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G38" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="10" t="s">
         <v>33</v>
       </c>
       <c r="I38" s="1" t="n">
@@ -2822,23 +2818,23 @@
       <c r="B39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="10" t="str">
+      <c r="C39" s="9" t="str">
         <f aca="false">IF(D39="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G39" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" s="11" t="s">
+      <c r="D39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G39" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I39" s="1" t="n">
@@ -2870,23 +2866,23 @@
       <c r="B40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="10" t="str">
+      <c r="C40" s="9" t="str">
         <f aca="false">IF(D40="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G40" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H40" s="11" t="s">
+      <c r="D40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G40" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I40" s="1" t="n">
@@ -2918,23 +2914,23 @@
       <c r="B41" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="10" t="str">
+      <c r="C41" s="9" t="str">
         <f aca="false">IF(D41="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G41" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H41" s="11" t="s">
+      <c r="D41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>39</v>
       </c>
       <c r="I41" s="1" t="n">
@@ -2966,23 +2962,23 @@
       <c r="B42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="13" t="str">
+      <c r="C42" s="12" t="str">
         <f aca="false">IF(D42="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G42" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" s="14" t="s">
+      <c r="D42" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G42" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I42" s="1" t="n">
@@ -3014,23 +3010,23 @@
       <c r="B43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="13" t="str">
+      <c r="C43" s="12" t="str">
         <f aca="false">IF(D43="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G43" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" s="14" t="s">
+      <c r="D43" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G43" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I43" s="1" t="n">
@@ -3062,23 +3058,23 @@
       <c r="B44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="13" t="str">
+      <c r="C44" s="12" t="str">
         <f aca="false">IF(D44="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G44" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" s="14" t="s">
+      <c r="D44" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G44" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I44" s="1" t="n">
@@ -3110,23 +3106,23 @@
       <c r="B45" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="13" t="str">
+      <c r="C45" s="12" t="str">
         <f aca="false">IF(D45="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E45" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G45" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H45" s="14" t="s">
+      <c r="D45" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G45" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I45" s="1" t="n">
@@ -3158,23 +3154,23 @@
       <c r="B46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="13" t="str">
+      <c r="C46" s="12" t="str">
         <f aca="false">IF(D46="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G46" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H46" s="14" t="s">
+      <c r="D46" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G46" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I46" s="1" t="n">
@@ -3206,23 +3202,23 @@
       <c r="B47" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="13" t="str">
+      <c r="C47" s="12" t="str">
         <f aca="false">IF(D47="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G47" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H47" s="14" t="s">
+      <c r="D47" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G47" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I47" s="1" t="n">
@@ -3254,23 +3250,23 @@
       <c r="B48" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="13" t="str">
+      <c r="C48" s="12" t="str">
         <f aca="false">IF(D48="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G48" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H48" s="14" t="s">
+      <c r="D48" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G48" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="13" t="s">
         <v>37</v>
       </c>
       <c r="I48" s="1" t="n">
@@ -3302,23 +3298,23 @@
       <c r="B49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="13" t="str">
+      <c r="C49" s="12" t="str">
         <f aca="false">IF(D49="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G49" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H49" s="14" t="s">
+      <c r="D49" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G49" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="13" t="s">
         <v>39</v>
       </c>
       <c r="I49" s="1" t="n">
@@ -3350,23 +3346,23 @@
       <c r="B50" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="7" t="str">
+      <c r="C50" s="6" t="str">
         <f aca="false">IF(D50="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E50" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G50" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H50" s="8" t="s">
+      <c r="D50" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G50" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I50" s="1" t="n">
@@ -3398,23 +3394,23 @@
       <c r="B51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="7" t="str">
+      <c r="C51" s="6" t="str">
         <f aca="false">IF(D51="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E51" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51" s="8" t="s">
+      <c r="D51" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G51" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I51" s="1" t="n">
@@ -3446,23 +3442,23 @@
       <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="7" t="str">
+      <c r="C52" s="6" t="str">
         <f aca="false">IF(D52="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E52" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G52" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" s="8" t="s">
+      <c r="D52" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G52" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I52" s="1" t="n">
@@ -3494,23 +3490,23 @@
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="7" t="str">
+      <c r="C53" s="6" t="str">
         <f aca="false">IF(D53="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G53" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" s="8" t="s">
+      <c r="D53" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G53" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I53" s="1" t="n">
@@ -3542,23 +3538,23 @@
       <c r="B54" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="7" t="str">
+      <c r="C54" s="6" t="str">
         <f aca="false">IF(D54="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E54" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" s="8" t="s">
+      <c r="D54" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G54" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I54" s="1" t="n">
@@ -3590,23 +3586,23 @@
       <c r="B55" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="7" t="str">
+      <c r="C55" s="6" t="str">
         <f aca="false">IF(D55="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G55" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" s="8" t="s">
+      <c r="D55" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G55" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I55" s="1" t="n">
@@ -3638,23 +3634,23 @@
       <c r="B56" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="7" t="str">
+      <c r="C56" s="6" t="str">
         <f aca="false">IF(D56="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E56" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G56" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H56" s="8" t="s">
+      <c r="D56" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G56" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I56" s="1" t="n">
@@ -3686,23 +3682,23 @@
       <c r="B57" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="7" t="str">
+      <c r="C57" s="6" t="str">
         <f aca="false">IF(D57="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E57" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G57" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H57" s="8" t="s">
+      <c r="D57" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G57" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="7" t="s">
         <v>39</v>
       </c>
       <c r="I57" s="1" t="n">
@@ -3734,23 +3730,23 @@
       <c r="B58" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="10" t="str">
+      <c r="C58" s="9" t="str">
         <f aca="false">IF(D58="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F58" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G58" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" s="11" t="s">
+      <c r="D58" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I58" s="1" t="n">
@@ -3782,23 +3778,23 @@
       <c r="B59" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="10" t="str">
+      <c r="C59" s="9" t="str">
         <f aca="false">IF(D59="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E59" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F59" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G59" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" s="11" t="s">
+      <c r="D59" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="10" t="s">
         <v>27</v>
       </c>
       <c r="I59" s="1" t="n">
@@ -3830,23 +3826,23 @@
       <c r="B60" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="10" t="str">
+      <c r="C60" s="9" t="str">
         <f aca="false">IF(D60="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E60" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F60" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G60" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" s="11" t="s">
+      <c r="D60" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G60" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="10" t="s">
         <v>29</v>
       </c>
       <c r="I60" s="1" t="n">
@@ -3878,23 +3874,23 @@
       <c r="B61" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="10" t="str">
+      <c r="C61" s="9" t="str">
         <f aca="false">IF(D61="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D61" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E61" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F61" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G61" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" s="11" t="s">
+      <c r="D61" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I61" s="1" t="n">
@@ -3926,23 +3922,23 @@
       <c r="B62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C62" s="10" t="str">
+      <c r="C62" s="9" t="str">
         <f aca="false">IF(D62="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F62" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G62" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" s="11" t="s">
+      <c r="D62" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G62" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="10" t="s">
         <v>33</v>
       </c>
       <c r="I62" s="1" t="n">
@@ -3974,23 +3970,23 @@
       <c r="B63" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C63" s="10" t="str">
+      <c r="C63" s="9" t="str">
         <f aca="false">IF(D63="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D63" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E63" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F63" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G63" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H63" s="11" t="s">
+      <c r="D63" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G63" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I63" s="1" t="n">
@@ -4022,23 +4018,23 @@
       <c r="B64" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="10" t="str">
+      <c r="C64" s="9" t="str">
         <f aca="false">IF(D64="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E64" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F64" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G64" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" s="11" t="s">
+      <c r="D64" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G64" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I64" s="1" t="n">
@@ -4070,23 +4066,23 @@
       <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="10" t="str">
+      <c r="C65" s="9" t="str">
         <f aca="false">IF(D65="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E65" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F65" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G65" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H65" s="11" t="s">
+      <c r="D65" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E65" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G65" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="10" t="s">
         <v>39</v>
       </c>
       <c r="I65" s="1" t="n">
@@ -4118,23 +4114,23 @@
       <c r="B66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="13" t="str">
+      <c r="C66" s="12" t="str">
         <f aca="false">IF(D66="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D66" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F66" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G66" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H66" s="14" t="s">
+      <c r="D66" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F66" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G66" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I66" s="1" t="n">
@@ -4166,23 +4162,23 @@
       <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="13" t="str">
+      <c r="C67" s="12" t="str">
         <f aca="false">IF(D67="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D67" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E67" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F67" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G67" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H67" s="14" t="s">
+      <c r="D67" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F67" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G67" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I67" s="1" t="n">
@@ -4214,23 +4210,23 @@
       <c r="B68" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="13" t="str">
+      <c r="C68" s="12" t="str">
         <f aca="false">IF(D68="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D68" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E68" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F68" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G68" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H68" s="14" t="s">
+      <c r="D68" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E68" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F68" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G68" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I68" s="1" t="n">
@@ -4262,23 +4258,23 @@
       <c r="B69" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="13" t="str">
+      <c r="C69" s="12" t="str">
         <f aca="false">IF(D69="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D69" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E69" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F69" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G69" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H69" s="14" t="s">
+      <c r="D69" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F69" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G69" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I69" s="1" t="n">
@@ -4310,23 +4306,23 @@
       <c r="B70" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C70" s="13" t="str">
+      <c r="C70" s="12" t="str">
         <f aca="false">IF(D70="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D70" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E70" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F70" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G70" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H70" s="14" t="s">
+      <c r="D70" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F70" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G70" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I70" s="1" t="n">
@@ -4358,23 +4354,23 @@
       <c r="B71" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="13" t="str">
+      <c r="C71" s="12" t="str">
         <f aca="false">IF(D71="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D71" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F71" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G71" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H71" s="14" t="s">
+      <c r="D71" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F71" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G71" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I71" s="1" t="n">
@@ -4406,23 +4402,23 @@
       <c r="B72" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C72" s="13" t="str">
+      <c r="C72" s="12" t="str">
         <f aca="false">IF(D72="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E72" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F72" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G72" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H72" s="14" t="s">
+      <c r="D72" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F72" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G72" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="13" t="s">
         <v>37</v>
       </c>
       <c r="I72" s="1" t="n">
@@ -4454,23 +4450,23 @@
       <c r="B73" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="13" t="str">
+      <c r="C73" s="12" t="str">
         <f aca="false">IF(D73="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D73" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E73" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F73" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G73" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H73" s="14" t="s">
+      <c r="D73" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F73" s="12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G73" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="13" t="s">
         <v>39</v>
       </c>
       <c r="I73" s="1" t="n">
@@ -4502,23 +4498,23 @@
       <c r="B74" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C74" s="7" t="str">
+      <c r="C74" s="6" t="str">
         <f aca="false">IF(D74="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E74" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F74" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H74" s="8" t="s">
+      <c r="D74" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F74" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G74" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I74" s="1" t="n">
@@ -4550,23 +4546,23 @@
       <c r="B75" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="7" t="str">
+      <c r="C75" s="6" t="str">
         <f aca="false">IF(D75="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E75" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F75" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" s="8" t="s">
+      <c r="D75" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F75" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G75" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I75" s="1" t="n">
@@ -4598,23 +4594,23 @@
       <c r="B76" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="7" t="str">
+      <c r="C76" s="6" t="str">
         <f aca="false">IF(D76="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E76" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F76" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G76" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H76" s="8" t="s">
+      <c r="D76" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F76" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I76" s="1" t="n">
@@ -4646,23 +4642,23 @@
       <c r="B77" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C77" s="7" t="str">
+      <c r="C77" s="6" t="str">
         <f aca="false">IF(D77="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E77" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F77" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G77" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H77" s="8" t="s">
+      <c r="D77" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E77" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F77" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G77" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I77" s="1" t="n">
@@ -4694,23 +4690,23 @@
       <c r="B78" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="7" t="str">
+      <c r="C78" s="6" t="str">
         <f aca="false">IF(D78="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E78" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F78" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G78" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H78" s="8" t="s">
+      <c r="D78" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E78" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F78" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G78" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I78" s="1" t="n">
@@ -4742,23 +4738,23 @@
       <c r="B79" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C79" s="7" t="str">
+      <c r="C79" s="6" t="str">
         <f aca="false">IF(D79="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E79" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F79" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G79" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H79" s="8" t="s">
+      <c r="D79" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F79" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G79" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I79" s="1" t="n">
@@ -4790,23 +4786,23 @@
       <c r="B80" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C80" s="7" t="str">
+      <c r="C80" s="6" t="str">
         <f aca="false">IF(D80="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E80" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F80" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G80" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H80" s="8" t="s">
+      <c r="D80" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E80" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F80" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G80" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I80" s="1" t="n">
@@ -4838,23 +4834,23 @@
       <c r="B81" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C81" s="7" t="str">
+      <c r="C81" s="6" t="str">
         <f aca="false">IF(D81="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E81" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F81" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="G81" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H81" s="8" t="s">
+      <c r="D81" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F81" s="6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G81" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" s="7" t="s">
         <v>39</v>
       </c>
       <c r="I81" s="1" t="n">
@@ -4886,23 +4882,23 @@
       <c r="B82" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C82" s="10" t="str">
+      <c r="C82" s="9" t="str">
         <f aca="false">IF(D82="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E82" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F82" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H82" s="11" t="s">
+      <c r="D82" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E82" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F82" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G82" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I82" s="1" t="n">
@@ -4934,23 +4930,23 @@
       <c r="B83" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C83" s="10" t="str">
+      <c r="C83" s="9" t="str">
         <f aca="false">IF(D83="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E83" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F83" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G83" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H83" s="11" t="s">
+      <c r="D83" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E83" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F83" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" s="10" t="s">
         <v>27</v>
       </c>
       <c r="I83" s="1" t="n">
@@ -4982,23 +4978,23 @@
       <c r="B84" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="10" t="str">
+      <c r="C84" s="9" t="str">
         <f aca="false">IF(D84="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D84" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E84" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F84" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G84" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H84" s="11" t="s">
+      <c r="D84" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F84" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G84" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="10" t="s">
         <v>29</v>
       </c>
       <c r="I84" s="1" t="n">
@@ -5030,23 +5026,23 @@
       <c r="B85" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="10" t="str">
+      <c r="C85" s="9" t="str">
         <f aca="false">IF(D85="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E85" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F85" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G85" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H85" s="11" t="s">
+      <c r="D85" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F85" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I85" s="1" t="n">
@@ -5078,23 +5074,23 @@
       <c r="B86" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C86" s="10" t="str">
+      <c r="C86" s="9" t="str">
         <f aca="false">IF(D86="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D86" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E86" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F86" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G86" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H86" s="11" t="s">
+      <c r="D86" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F86" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G86" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" s="10" t="s">
         <v>33</v>
       </c>
       <c r="I86" s="1" t="n">
@@ -5126,23 +5122,23 @@
       <c r="B87" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C87" s="10" t="str">
+      <c r="C87" s="9" t="str">
         <f aca="false">IF(D87="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D87" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E87" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F87" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G87" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H87" s="11" t="s">
+      <c r="D87" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E87" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F87" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" s="10" t="s">
         <v>35</v>
       </c>
       <c r="I87" s="1" t="n">
@@ -5174,23 +5170,23 @@
       <c r="B88" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C88" s="10" t="str">
+      <c r="C88" s="9" t="str">
         <f aca="false">IF(D88="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D88" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E88" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F88" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H88" s="11" t="s">
+      <c r="D88" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F88" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G88" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I88" s="1" t="n">
@@ -5222,23 +5218,23 @@
       <c r="B89" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C89" s="10" t="str">
+      <c r="C89" s="9" t="str">
         <f aca="false">IF(D89="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D89" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E89" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="F89" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="G89" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H89" s="11" t="s">
+      <c r="D89" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E89" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F89" s="9" t="n">
+        <v>80000</v>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="10" t="s">
         <v>39</v>
       </c>
       <c r="I89" s="1" t="n">
@@ -5270,23 +5266,23 @@
       <c r="B90" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C90" s="13" t="str">
+      <c r="C90" s="12" t="str">
         <f aca="false">IF(D90="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D90" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E90" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F90" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G90" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H90" s="14" t="s">
+      <c r="D90" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F90" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G90" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I90" s="1" t="n">
@@ -5318,23 +5314,23 @@
       <c r="B91" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C91" s="13" t="str">
+      <c r="C91" s="12" t="str">
         <f aca="false">IF(D91="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D91" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E91" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F91" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G91" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H91" s="14" t="s">
+      <c r="D91" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E91" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F91" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G91" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H91" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I91" s="1" t="n">
@@ -5366,23 +5362,23 @@
       <c r="B92" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C92" s="13" t="str">
+      <c r="C92" s="12" t="str">
         <f aca="false">IF(D92="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D92" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E92" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F92" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G92" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H92" s="14" t="s">
+      <c r="D92" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F92" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G92" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" s="13" t="s">
         <v>29</v>
       </c>
       <c r="I92" s="1" t="n">
@@ -5414,23 +5410,23 @@
       <c r="B93" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C93" s="13" t="str">
+      <c r="C93" s="12" t="str">
         <f aca="false">IF(D93="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D93" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E93" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F93" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G93" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H93" s="14" t="s">
+      <c r="D93" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E93" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F93" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G93" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I93" s="1" t="n">
@@ -5462,23 +5458,23 @@
       <c r="B94" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C94" s="13" t="str">
+      <c r="C94" s="12" t="str">
         <f aca="false">IF(D94="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D94" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E94" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F94" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G94" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H94" s="14" t="s">
+      <c r="D94" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E94" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F94" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G94" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I94" s="1" t="n">
@@ -5510,23 +5506,23 @@
       <c r="B95" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C95" s="13" t="str">
+      <c r="C95" s="12" t="str">
         <f aca="false">IF(D95="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D95" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E95" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F95" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G95" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H95" s="14" t="s">
+      <c r="D95" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E95" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F95" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G95" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I95" s="1" t="n">
@@ -5558,23 +5554,23 @@
       <c r="B96" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C96" s="13" t="str">
+      <c r="C96" s="12" t="str">
         <f aca="false">IF(D96="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D96" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E96" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F96" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G96" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H96" s="14" t="s">
+      <c r="D96" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F96" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G96" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H96" s="13" t="s">
         <v>37</v>
       </c>
       <c r="I96" s="1" t="n">
@@ -5606,23 +5602,23 @@
       <c r="B97" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C97" s="13" t="str">
+      <c r="C97" s="12" t="str">
         <f aca="false">IF(D97="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D97" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E97" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F97" s="13" t="n">
-        <v>160</v>
-      </c>
-      <c r="G97" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H97" s="14" t="s">
+      <c r="D97" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E97" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F97" s="12" t="n">
+        <v>160000</v>
+      </c>
+      <c r="G97" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H97" s="13" t="s">
         <v>39</v>
       </c>
       <c r="I97" s="1" t="n">
@@ -5654,23 +5650,23 @@
       <c r="B98" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C98" s="7" t="str">
+      <c r="C98" s="6" t="str">
         <f aca="false">IF(D98="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E98" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F98" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H98" s="8" t="s">
+      <c r="D98" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E98" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F98" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G98" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H98" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I98" s="1" t="n">
@@ -5702,23 +5698,23 @@
       <c r="B99" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="7" t="str">
+      <c r="C99" s="6" t="str">
         <f aca="false">IF(D99="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D99" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E99" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F99" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H99" s="8" t="s">
+      <c r="D99" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E99" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F99" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G99" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I99" s="1" t="n">
@@ -5750,23 +5746,23 @@
       <c r="B100" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C100" s="7" t="str">
+      <c r="C100" s="6" t="str">
         <f aca="false">IF(D100="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E100" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F100" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H100" s="8" t="s">
+      <c r="D100" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E100" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F100" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G100" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H100" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I100" s="1" t="n">
@@ -5798,23 +5794,23 @@
       <c r="B101" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C101" s="7" t="str">
+      <c r="C101" s="6" t="str">
         <f aca="false">IF(D101="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D101" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E101" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F101" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H101" s="8" t="s">
+      <c r="D101" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E101" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F101" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G101" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H101" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I101" s="1" t="n">
@@ -5846,23 +5842,23 @@
       <c r="B102" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C102" s="7" t="str">
+      <c r="C102" s="6" t="str">
         <f aca="false">IF(D102="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E102" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F102" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H102" s="8" t="s">
+      <c r="D102" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E102" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F102" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G102" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H102" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I102" s="1" t="n">
@@ -5894,23 +5890,23 @@
       <c r="B103" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C103" s="7" t="str">
+      <c r="C103" s="6" t="str">
         <f aca="false">IF(D103="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E103" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F103" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H103" s="8" t="s">
+      <c r="D103" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E103" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F103" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G103" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H103" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I103" s="1" t="n">
@@ -5942,23 +5938,23 @@
       <c r="B104" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C104" s="7" t="str">
+      <c r="C104" s="6" t="str">
         <f aca="false">IF(D104="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E104" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F104" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H104" s="8" t="s">
+      <c r="D104" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E104" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F104" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G104" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H104" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I104" s="1" t="n">
@@ -5990,23 +5986,23 @@
       <c r="B105" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C105" s="7" t="str">
+      <c r="C105" s="6" t="str">
         <f aca="false">IF(D105="OnDemand","ExperimentA","ExperimentB")</f>
         <v>ExperimentB</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E105" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="F105" s="7" t="n">
-        <v>320</v>
-      </c>
-      <c r="G105" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H105" s="8" t="s">
+      <c r="D105" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E105" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="F105" s="6" t="n">
+        <v>320000</v>
+      </c>
+      <c r="G105" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" s="7" t="s">
         <v>39</v>
       </c>
       <c r="I105" s="1" t="n">

</xml_diff>